<commit_message>
knn, decision tree, centroid, svm
</commit_message>
<xml_diff>
--- a/Accuracy.xlsx
+++ b/Accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h337\project\E4012_rastliny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4302E877-837C-408C-967D-773D3D8541A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11857087-B775-48DB-B519-7C18FFE54C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8BECC03F-F93F-48DD-891A-0437997CB34F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Model</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>DT (5)</t>
+  </si>
+  <si>
+    <t>centroid</t>
+  </si>
+  <si>
+    <t>SVM</t>
   </si>
 </sst>
 </file>
@@ -412,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293B6116-94B6-41C7-8C15-AE0BDFBBA792}">
-  <dimension ref="A2:E5"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,6 +500,40 @@
         <v>0.97</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.88600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="D7">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="E7">
+        <v>0.96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>